<commit_message>
Compliance: Update Pi-Connect Lite
</commit_message>
<xml_diff>
--- a/Compliance/EN 50581/PiConnectLite.xlsx
+++ b/Compliance/EN 50581/PiConnectLite.xlsx
@@ -10,12 +10,12 @@
     <sheet name="PiConnectLite" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="199">
   <si>
     <t>Item</t>
   </si>
@@ -62,18 +62,12 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>0.1uF, 16V</t>
   </si>
   <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>CC0805KRX7R7BB104</t>
-  </si>
-  <si>
     <t>311-1142-1-ND</t>
   </si>
   <si>
@@ -110,12 +104,6 @@
     <t>2.2UF-25V</t>
   </si>
   <si>
-    <t>CC0805KKX7R8BB225</t>
-  </si>
-  <si>
-    <t>311-1884-1-ND</t>
-  </si>
-  <si>
     <t>OPL</t>
   </si>
   <si>
@@ -134,18 +122,12 @@
     <t>1276-1285-1-ND</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>KEMET</t>
   </si>
   <si>
     <t>C0603C104Z4VACTU</t>
   </si>
   <si>
-    <t>399-1098-1-ND</t>
-  </si>
-  <si>
     <t>C13</t>
   </si>
   <si>
@@ -194,12 +176,6 @@
     <t>Lite-On Inc.</t>
   </si>
   <si>
-    <t>LTST-C190GKT</t>
-  </si>
-  <si>
-    <t>160-1183-1-ND</t>
-  </si>
-  <si>
     <t>D3</t>
   </si>
   <si>
@@ -422,12 +398,6 @@
     <t>11.8K</t>
   </si>
   <si>
-    <t>CRCW040211K8FKED</t>
-  </si>
-  <si>
-    <t>541-11.8KLCT-ND</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
@@ -608,9 +578,6 @@
     <t>http://www.vishay.com/product?docid=34313&amp;tab=quality</t>
   </si>
   <si>
-    <t>https://api.kemet.com/component-edge/download/rohs/C0603C104Z4VACTU.pdf</t>
-  </si>
-  <si>
     <t>https://api.kemet.com/component-edge/download/rohs/C0805C751J5GACTU.pdf</t>
   </si>
   <si>
@@ -618,13 +585,40 @@
   </si>
   <si>
     <t>https://www.ckswitches.com/wp-content/uploads/2019/10/rohs-reach-compliance-certificate.pdf</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM155R61A225KE95D</t>
+  </si>
+  <si>
+    <t>RC0402FR-0711K8L</t>
+  </si>
+  <si>
+    <t>C2, C12</t>
+  </si>
+  <si>
+    <t>490-10451-1-ND</t>
+  </si>
+  <si>
+    <t>YAG2958CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/en-eu/support/compliance/rohs</t>
+  </si>
+  <si>
+    <t>LTST-S270GKT</t>
+  </si>
+  <si>
+    <t>160-1475-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,6 +754,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1058,7 +1060,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1101,11 +1103,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1139,6 +1143,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1157,6 +1162,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M35" totalsRowShown="0">
+  <autoFilter ref="A1:M35"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Item"/>
+    <tableColumn id="2" name="Qty"/>
+    <tableColumn id="3" name="Reference(s)"/>
+    <tableColumn id="4" name="Value"/>
+    <tableColumn id="5" name="MFR"/>
+    <tableColumn id="6" name="MPN"/>
+    <tableColumn id="7" name="Max Temp (C)"/>
+    <tableColumn id="8" name="Min Temp (C)"/>
+    <tableColumn id="9" name="SPN"/>
+    <tableColumn id="10" name="SPR"/>
+    <tableColumn id="11" name="ROHS Compliant?"/>
+    <tableColumn id="12" name="ROHS Compatible?"/>
+    <tableColumn id="13" name="Supplier Declaration"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1446,85 +1473,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M37"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="246" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" t="s">
+        <v>157</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>125</v>
+      </c>
+      <c r="H2">
+        <v>-55</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>165</v>
-      </c>
-      <c r="L2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="M2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>125</v>
@@ -1533,147 +1599,150 @@
         <v>-55</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="H4">
         <v>-55</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M4" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G5">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="H5">
         <v>-55</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
         <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M5" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>191</v>
       </c>
       <c r="G6">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="H6">
         <v>-55</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>194</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M6" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G7">
         <v>125</v>
@@ -1682,36 +1751,36 @@
         <v>-55</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M7" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G8">
         <v>125</v>
@@ -1720,282 +1789,282 @@
         <v>-55</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
         <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M8" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G9">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="H9">
-        <v>-30</v>
+        <v>-55</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s">
         <v>14</v>
       </c>
       <c r="K9" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M9" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G10">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H10">
-        <v>-55</v>
+        <v>-40</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J10" t="s">
         <v>14</v>
       </c>
       <c r="K10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M10" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
       <c r="G11">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="H11">
         <v>-55</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
       <c r="J11" t="s">
         <v>14</v>
       </c>
       <c r="K11" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M11" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G12">
         <v>150</v>
       </c>
       <c r="H12">
-        <v>-40</v>
+        <v>-65</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
         <v>14</v>
       </c>
       <c r="K12" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="M12" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G13">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="H13">
-        <v>-55</v>
+        <v>-65</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
         <v>14</v>
       </c>
       <c r="K13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M13" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G14">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="H14">
-        <v>-65</v>
+        <v>-40</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J14" t="s">
         <v>14</v>
       </c>
       <c r="K14" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M14" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G15">
-        <v>150</v>
+        <v>85</v>
       </c>
       <c r="H15">
-        <v>-65</v>
+        <v>-25</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J15" t="s">
         <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M15" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2006,215 +2075,215 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16">
-        <v>105</v>
-      </c>
-      <c r="H16">
-        <v>-40</v>
+        <v>75</v>
+      </c>
+      <c r="F16">
+        <v>1053131102</v>
       </c>
       <c r="I16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J16" t="s">
         <v>14</v>
       </c>
       <c r="K16" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M16" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G17">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="H17">
-        <v>-25</v>
+        <v>-55</v>
       </c>
       <c r="I17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s">
         <v>14</v>
       </c>
       <c r="K17" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="M17" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F18">
-        <v>1053131102</v>
+        <v>744383230047</v>
+      </c>
+      <c r="G18">
+        <v>125</v>
+      </c>
+      <c r="H18">
+        <v>-40</v>
       </c>
       <c r="I18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J18" t="s">
         <v>14</v>
       </c>
       <c r="K18" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M18" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G19">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H19">
         <v>-55</v>
       </c>
       <c r="I19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J19" t="s">
         <v>14</v>
       </c>
       <c r="K19" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="M19" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20">
-        <v>744383230047</v>
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
       </c>
       <c r="G20">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H20">
-        <v>-40</v>
+        <v>-55</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="K20" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M20" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
         <v>95</v>
       </c>
       <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
         <v>96</v>
       </c>
-      <c r="F21" t="s">
-        <v>97</v>
-      </c>
       <c r="G21">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="H21">
         <v>-55</v>
       </c>
       <c r="I21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="K21" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M21" t="s">
         <v>173</v>
@@ -2222,37 +2291,37 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
         <v>99</v>
       </c>
-      <c r="D22" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" t="s">
-        <v>101</v>
-      </c>
       <c r="G22">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="H22">
         <v>-55</v>
       </c>
       <c r="I22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K22" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M22" t="s">
         <v>173</v>
@@ -2260,22 +2329,22 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
         <v>103</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" t="s">
-        <v>104</v>
       </c>
       <c r="G23">
         <v>155</v>
@@ -2284,39 +2353,39 @@
         <v>-55</v>
       </c>
       <c r="I23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K23" t="s">
-        <v>168</v>
-      </c>
-      <c r="M23" t="s">
-        <v>183</v>
+        <v>158</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
         <v>106</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s">
         <v>107</v>
       </c>
       <c r="G24">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="H24">
         <v>-55</v>
@@ -2325,18 +2394,18 @@
         <v>108</v>
       </c>
       <c r="J24" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K24" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M24" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2348,7 +2417,7 @@
         <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
         <v>111</v>
@@ -2363,18 +2432,18 @@
         <v>112</v>
       </c>
       <c r="J25" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K25" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2386,48 +2455,48 @@
         <v>114</v>
       </c>
       <c r="E26" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="F26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G26">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="H26">
         <v>-55</v>
       </c>
       <c r="I26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J26" t="s">
         <v>14</v>
       </c>
       <c r="K26" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M26" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G27">
         <v>155</v>
@@ -2436,36 +2505,36 @@
         <v>-55</v>
       </c>
       <c r="I27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J27" t="s">
         <v>14</v>
       </c>
       <c r="K27" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="M27" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" t="s">
         <v>122</v>
       </c>
+      <c r="D28">
+        <v>300</v>
+      </c>
       <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="s">
         <v>123</v>
-      </c>
-      <c r="F28" t="s">
-        <v>124</v>
       </c>
       <c r="G28">
         <v>155</v>
@@ -2474,36 +2543,36 @@
         <v>-55</v>
       </c>
       <c r="I28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J28" t="s">
         <v>14</v>
       </c>
       <c r="K28" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="M28" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
         <v>126</v>
       </c>
-      <c r="D29" t="s">
-        <v>127</v>
-      </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="G29">
         <v>155</v>
@@ -2512,80 +2581,83 @@
         <v>-55</v>
       </c>
       <c r="I29" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="J29" t="s">
         <v>14</v>
       </c>
       <c r="K29" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="M29" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" t="s">
         <v>130</v>
       </c>
-      <c r="D30">
-        <v>300</v>
-      </c>
-      <c r="E30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="G30">
+        <v>70</v>
+      </c>
+      <c r="H30">
+        <v>-30</v>
+      </c>
+      <c r="I30" t="s">
         <v>131</v>
       </c>
-      <c r="G30">
-        <v>155</v>
-      </c>
-      <c r="H30">
-        <v>-55</v>
-      </c>
-      <c r="I30" t="s">
-        <v>132</v>
-      </c>
       <c r="J30" t="s">
         <v>14</v>
       </c>
       <c r="K30" t="s">
+        <v>158</v>
+      </c>
+      <c r="L30" t="s">
         <v>168</v>
       </c>
       <c r="M30" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" t="s">
         <v>133</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>134</v>
-      </c>
-      <c r="E31" t="s">
-        <v>87</v>
       </c>
       <c r="F31" t="s">
         <v>135</v>
       </c>
       <c r="G31">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="H31">
-        <v>-55</v>
+        <v>-40</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
@@ -2594,15 +2666,15 @@
         <v>14</v>
       </c>
       <c r="K31" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="M31" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2614,225 +2686,146 @@
         <v>138</v>
       </c>
       <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
         <v>139</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32">
+        <v>125</v>
+      </c>
+      <c r="H32">
+        <v>-40</v>
+      </c>
+      <c r="I32" t="s">
         <v>140</v>
       </c>
-      <c r="G32">
-        <v>70</v>
-      </c>
-      <c r="H32">
-        <v>-30</v>
-      </c>
-      <c r="I32" t="s">
-        <v>141</v>
-      </c>
       <c r="J32" t="s">
         <v>14</v>
       </c>
       <c r="K32" t="s">
-        <v>168</v>
-      </c>
-      <c r="L32" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="M32" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" t="s">
         <v>142</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>143</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>144</v>
       </c>
-      <c r="F33" t="s">
-        <v>145</v>
-      </c>
       <c r="G33">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="H33">
         <v>-40</v>
       </c>
       <c r="I33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J33" t="s">
         <v>14</v>
       </c>
       <c r="K33" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M33" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" t="s">
         <v>147</v>
       </c>
-      <c r="D34" t="s">
-        <v>148</v>
-      </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="F34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G34">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="H34">
         <v>-40</v>
       </c>
       <c r="I34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J34" t="s">
         <v>14</v>
       </c>
       <c r="K34" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" t="s">
+        <v>150</v>
+      </c>
+      <c r="I35" t="s">
         <v>151</v>
       </c>
-      <c r="D35" t="s">
-        <v>152</v>
-      </c>
-      <c r="E35" t="s">
-        <v>153</v>
-      </c>
-      <c r="F35" t="s">
-        <v>154</v>
-      </c>
-      <c r="G35">
-        <v>125</v>
-      </c>
-      <c r="H35">
-        <v>-40</v>
-      </c>
-      <c r="I35" t="s">
-        <v>155</v>
-      </c>
       <c r="J35" t="s">
         <v>14</v>
       </c>
       <c r="K35" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M35" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" t="s">
-        <v>157</v>
-      </c>
-      <c r="E36" t="s">
-        <v>153</v>
-      </c>
-      <c r="F36" t="s">
-        <v>157</v>
-      </c>
-      <c r="G36">
-        <v>150</v>
-      </c>
-      <c r="H36">
-        <v>-40</v>
-      </c>
-      <c r="I36" t="s">
-        <v>158</v>
-      </c>
-      <c r="J36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K36" t="s">
-        <v>168</v>
-      </c>
-      <c r="M36" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>39</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
-      </c>
-      <c r="D37" t="s">
-        <v>160</v>
-      </c>
-      <c r="E37" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" t="s">
-        <v>160</v>
-      </c>
-      <c r="G37">
-        <v>85</v>
-      </c>
-      <c r="H37">
-        <v>-40</v>
-      </c>
-      <c r="I37" t="s">
-        <v>161</v>
-      </c>
-      <c r="J37" t="s">
-        <v>14</v>
-      </c>
-      <c r="K37" t="s">
-        <v>168</v>
-      </c>
-      <c r="M37" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2851,24 +2844,24 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pi-Connect Lite: Change Q1 with more efficient FET
</commit_message>
<xml_diff>
--- a/Compliance/EN 50581/PiConnectLite.xlsx
+++ b/Compliance/EN 50581/PiConnectLite.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="200">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -365,22 +365,25 @@
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">DMMT5401</t>
+    <t xml:space="preserve">SI2323DDS-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay Siliconix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI2323DDS-T1-GE3CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.vishay.com/docs/99912/mat_cat_policy.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMG2305UX</t>
   </si>
   <si>
     <t xml:space="preserve">DiodesZetex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMMT5401-7-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMMT5401-FDICT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMG2305UX</t>
   </si>
   <si>
     <t xml:space="preserve">DMG2305UX-7</t>
@@ -758,11 +761,11 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.72"/>
@@ -1458,7 +1461,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>115</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>150</v>
@@ -1484,16 +1487,16 @@
         <v>-55</v>
       </c>
       <c r="I19" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,10 +1513,10 @@
         <v>119</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>150</v>
@@ -1522,10 +1525,10 @@
         <v>-55</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K20" s="0" t="s">
         <v>19</v>
@@ -1542,16 +1545,16 @@
         <v>4</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>155</v>
@@ -1560,16 +1563,16 @@
         <v>-55</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>19</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,16 +1583,16 @@
         <v>2</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>155</v>
@@ -1598,16 +1601,16 @@
         <v>-55</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,16 +1621,16 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>155</v>
@@ -1636,16 +1639,16 @@
         <v>-55</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>19</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,16 +1659,16 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>29</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>125</v>
@@ -1674,7 +1677,7 @@
         <v>-55</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>18</v>
@@ -1683,7 +1686,7 @@
         <v>19</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,16 +1697,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>104</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>155</v>
@@ -1712,7 +1715,7 @@
         <v>-55</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>18</v>
@@ -1721,7 +1724,7 @@
         <v>65</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,16 +1735,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>155</v>
@@ -1750,7 +1753,7 @@
         <v>-55</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J26" s="0" t="s">
         <v>18</v>
@@ -1759,7 +1762,7 @@
         <v>65</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,16 +1773,16 @@
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>104</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>155</v>
@@ -1788,7 +1791,7 @@
         <v>-55</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J27" s="0" t="s">
         <v>18</v>
@@ -1797,7 +1800,7 @@
         <v>65</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>300</v>
@@ -1817,7 +1820,7 @@
         <v>29</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>155</v>
@@ -1826,7 +1829,7 @@
         <v>-55</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J28" s="0" t="s">
         <v>18</v>
@@ -1835,7 +1838,7 @@
         <v>19</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>155</v>
@@ -1864,7 +1867,7 @@
         <v>-55</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>18</v>
@@ -1873,7 +1876,7 @@
         <v>19</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1884,16 +1887,16 @@
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>70</v>
@@ -1902,7 +1905,7 @@
         <v>-30</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J30" s="0" t="s">
         <v>18</v>
@@ -1911,10 +1914,10 @@
         <v>19</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,16 +1928,16 @@
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>85</v>
@@ -1943,7 +1946,7 @@
         <v>-40</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>18</v>
@@ -1952,7 +1955,7 @@
         <v>19</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,16 +1966,16 @@
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>75</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>125</v>
@@ -1981,7 +1984,7 @@
         <v>-40</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>18</v>
@@ -1990,7 +1993,7 @@
         <v>19</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2001,16 +2004,16 @@
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>125</v>
@@ -2019,7 +2022,7 @@
         <v>-40</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>18</v>
@@ -2028,7 +2031,7 @@
         <v>19</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,16 +2042,16 @@
         <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>85</v>
@@ -2057,7 +2060,7 @@
         <v>-40</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>18</v>
@@ -2066,7 +2069,7 @@
         <v>19</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,19 +2080,19 @@
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J35" s="0" t="s">
         <v>18</v>
@@ -2098,7 +2101,7 @@
         <v>19</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2129,31 +2132,31 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>